<commit_message>
Fixed bug, added print. Now works
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ну, это...</t>
+          <t xml:space="preserve">  А можете выделить какие у этих фигур есть признаки?  По которым они варьируются?  Признаки? Размер и метка.</t>
         </is>
       </c>
     </row>
@@ -456,7 +456,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> А не одинаковый, по...</t>
+          <t xml:space="preserve">  Размер и метка.  А еще какие-нибудь есть?  Нет.  Ну, это...  Они одинаковые по названию одной игрушки.</t>
         </is>
       </c>
     </row>
@@ -466,7 +466,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> А, у, от названия одной гучки.</t>
+          <t xml:space="preserve">  Одинаковый размер и метка.  А в принципе, ну, вот рандомная фигура, какие можно признаки выделить, если ее не относили к группе?</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Раз...</t>
+          <t xml:space="preserve">  А, чтобы в новую группу определить размер и присутствие или отсутствие метки.  А если не определять? Просто как абстрактная фигура?  Любая абстрактная фигура.</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,87 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> И одинаковое размеры и нет.</t>
+          <t xml:space="preserve">  Тут имеет значение только метка и размер фигуры, то есть масштаб признаков.  То есть тут есть маленькие фигуры.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Большие фигуры с меткой, большие фигуры без метки, большие фигуры с меткой и средние, хотя нет, это тоже, наверное, маленькие фигуры без метки.  Так...</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Дополнительные фигуры не вызывали сомнения, куда их определить?  Нет.  Вам помогали ваши профессиональные навыки?  Наверное, да. Не знаю.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Ммм...  А... Ну, что могло вам помочь?  Ну, классифицирование.  Угу.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Вы любите читать?  Ну, да.  А много читаете?  Когда как. Когда могу зачитываться, когда могу по углам читать.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Могу за месяц схавать 10 книг, а потом такой, ну, мне что-то нечего читать, ну ладно.  Вы решаете задачную логику?  Ну, скорее это, в принципе, как самоцель или как деятельность.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Ну, без разницы.  Ну, скорее всего, да. Потому что приходится.  Угу. Как вы думаете, там могло в</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Не знаю. Ну, в целом.  Есть ли какие-то комментарии к проведению эксперимента?  Ну, что-то не понравилось там.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Да.  Справить что-то можно. Нет?  В принципе, всё понятно.  Хотели бы ещё раз поучаствовать?  Да.  Всё, спасибо.</t>
         </is>
       </c>
     </row>

</xml_diff>